<commit_message>
Add latest submission and model details to xlsx file
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -44,16 +44,30 @@
   </si>
   <si>
     <t xml:space="preserve">learning_rate =0.1,
-    n_estimators=500,
-    max_depth=5,
-    min_child_weight=1,
-    gamma=0,
-    subsample=0.8,
-    colsample_bytree=0.8,
-    objective= 'multi:softprob',
-    nthread=4,
-    scale_pos_weight=1,
-    Seed=27</t>
+n_estimators=500,
+max_depth=5,
+min_child_weight=1,
+gamma=0,
+subsample=0.8,
+colsample_bytree=0.8,
+objective= 'multi:softprob',
+Nthread=4,
+scale_pos_weight=1,
+Seed=27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xgboost (All feature engineering done)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">booster=gbtree,
+objective=multi:softprob,
+num_class=9,
+eval_mtric=logloss,
+scale_pos_weight=1.0
+bst_eta=0.5,
+bst:max_depth=5,
+bst:colsample_bytree=0.5,
+Nthread=8</t>
   </si>
 </sst>
 </file>
@@ -63,11 +77,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -83,6 +98,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,12 +149,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -157,31 +183,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.9336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.3163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="24.0357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -203,7 +229,7 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -211,6 +237,20 @@
       </c>
       <c r="D3" s="1" t="n">
         <v>110</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.007380195</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>